<commit_message>
wheels, tires and kits are all finished
</commit_message>
<xml_diff>
--- a/sheets/WheelPros/wheel_pros_kits.xlsx
+++ b/sheets/WheelPros/wheel_pros_kits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary R. Jones\PycharmProjects\racks_deep\sheets\WheelPros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A85CF5D-BBB9-42D0-8A3D-906797E746E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC340FC1-151A-4785-8D09-D0917DC51FFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{ECDD2B8B-24B6-41DE-BF3A-13A829B24C26}"/>
+    <workbookView xWindow="6285" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{ECDD2B8B-24B6-41DE-BF3A-13A829B24C26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7077" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7078" uniqueCount="175">
   <si>
     <t>12" MSA Black/Machined Kits</t>
   </si>
@@ -554,6 +554,9 @@
   <si>
     <t>24x7</t>
   </si>
+  <si>
+    <t>Size</t>
+  </si>
 </sst>
 </file>
 
@@ -1011,7 +1014,7 @@
   <dimension ref="A1:F1838"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H1748" sqref="H1748"/>
+      <selection activeCell="F1726" sqref="F1726"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,6 +1042,9 @@
       <c r="E1" t="s">
         <v>164</v>
       </c>
+      <c r="F1" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -36401,349 +36407,211 @@
       </c>
     </row>
     <row r="1770" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1770" s="5">
-        <v>1769</v>
-      </c>
+      <c r="A1770" s="5"/>
     </row>
     <row r="1771" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1771" s="5">
-        <v>1770</v>
-      </c>
+      <c r="A1771" s="5"/>
     </row>
     <row r="1772" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1772" s="5">
-        <v>1771</v>
-      </c>
+      <c r="A1772" s="5"/>
     </row>
     <row r="1773" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1773" s="5">
-        <v>1772</v>
-      </c>
+      <c r="A1773" s="5"/>
     </row>
     <row r="1774" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1774" s="5">
-        <v>1773</v>
-      </c>
+      <c r="A1774" s="5"/>
     </row>
     <row r="1775" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1775" s="5">
-        <v>1774</v>
-      </c>
+      <c r="A1775" s="5"/>
     </row>
     <row r="1776" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1776" s="5">
-        <v>1775</v>
-      </c>
+      <c r="A1776" s="5"/>
     </row>
     <row r="1777" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1777" s="5">
-        <v>1776</v>
-      </c>
+      <c r="A1777" s="5"/>
     </row>
     <row r="1778" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1778" s="5">
-        <v>1777</v>
-      </c>
+      <c r="A1778" s="5"/>
     </row>
     <row r="1779" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1779" s="5">
-        <v>1778</v>
-      </c>
+      <c r="A1779" s="5"/>
     </row>
     <row r="1780" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1780" s="5">
-        <v>1779</v>
-      </c>
+      <c r="A1780" s="5"/>
     </row>
     <row r="1781" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1781" s="5">
-        <v>1780</v>
-      </c>
+      <c r="A1781" s="5"/>
     </row>
     <row r="1782" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1782" s="5">
-        <v>1781</v>
-      </c>
+      <c r="A1782" s="5"/>
     </row>
     <row r="1783" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1783" s="5">
-        <v>1782</v>
-      </c>
+      <c r="A1783" s="5"/>
     </row>
     <row r="1784" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1784" s="5">
-        <v>1783</v>
-      </c>
+      <c r="A1784" s="5"/>
     </row>
     <row r="1785" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1785" s="5">
-        <v>1784</v>
-      </c>
+      <c r="A1785" s="5"/>
     </row>
     <row r="1786" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1786" s="5">
-        <v>1785</v>
-      </c>
+      <c r="A1786" s="5"/>
     </row>
     <row r="1787" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1787" s="5">
-        <v>1786</v>
-      </c>
+      <c r="A1787" s="5"/>
     </row>
     <row r="1788" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1788" s="5">
-        <v>1787</v>
-      </c>
+      <c r="A1788" s="5"/>
     </row>
     <row r="1789" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1789" s="5">
-        <v>1788</v>
-      </c>
+      <c r="A1789" s="5"/>
     </row>
     <row r="1790" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1790" s="5">
-        <v>1789</v>
-      </c>
+      <c r="A1790" s="5"/>
     </row>
     <row r="1791" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1791" s="5">
-        <v>1790</v>
-      </c>
+      <c r="A1791" s="5"/>
     </row>
     <row r="1792" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1792" s="5">
-        <v>1791</v>
-      </c>
+      <c r="A1792" s="5"/>
     </row>
     <row r="1793" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1793" s="5">
-        <v>1792</v>
-      </c>
+      <c r="A1793" s="5"/>
     </row>
     <row r="1794" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1794" s="5">
-        <v>1793</v>
-      </c>
+      <c r="A1794" s="5"/>
     </row>
     <row r="1795" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1795" s="5">
-        <v>1794</v>
-      </c>
+      <c r="A1795" s="5"/>
     </row>
     <row r="1796" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1796" s="5">
-        <v>1795</v>
-      </c>
+      <c r="A1796" s="5"/>
     </row>
     <row r="1797" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1797" s="5">
-        <v>1796</v>
-      </c>
+      <c r="A1797" s="5"/>
     </row>
     <row r="1798" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1798" s="5">
-        <v>1797</v>
-      </c>
+      <c r="A1798" s="5"/>
     </row>
     <row r="1799" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1799" s="5">
-        <v>1798</v>
-      </c>
+      <c r="A1799" s="5"/>
     </row>
     <row r="1800" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1800" s="5">
-        <v>1799</v>
-      </c>
+      <c r="A1800" s="5"/>
     </row>
     <row r="1801" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1801" s="5">
-        <v>1800</v>
-      </c>
+      <c r="A1801" s="5"/>
     </row>
     <row r="1802" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1802" s="5">
-        <v>1801</v>
-      </c>
+      <c r="A1802" s="5"/>
     </row>
     <row r="1803" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1803" s="5">
-        <v>1802</v>
-      </c>
+      <c r="A1803" s="5"/>
     </row>
     <row r="1804" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1804" s="5">
-        <v>1803</v>
-      </c>
+      <c r="A1804" s="5"/>
     </row>
     <row r="1805" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1805" s="5">
-        <v>1804</v>
-      </c>
+      <c r="A1805" s="5"/>
     </row>
     <row r="1806" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1806" s="5">
-        <v>1805</v>
-      </c>
+      <c r="A1806" s="5"/>
     </row>
     <row r="1807" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1807" s="5">
-        <v>1806</v>
-      </c>
+      <c r="A1807" s="5"/>
     </row>
     <row r="1808" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1808" s="5">
-        <v>1807</v>
-      </c>
+      <c r="A1808" s="5"/>
     </row>
     <row r="1809" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1809" s="5">
-        <v>1808</v>
-      </c>
+      <c r="A1809" s="5"/>
     </row>
     <row r="1810" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1810" s="5">
-        <v>1809</v>
-      </c>
+      <c r="A1810" s="5"/>
     </row>
     <row r="1811" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1811" s="5">
-        <v>1810</v>
-      </c>
+      <c r="A1811" s="5"/>
     </row>
     <row r="1812" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1812" s="5">
-        <v>1811</v>
-      </c>
+      <c r="A1812" s="5"/>
     </row>
     <row r="1813" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1813" s="5">
-        <v>1812</v>
-      </c>
+      <c r="A1813" s="5"/>
     </row>
     <row r="1814" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1814" s="5">
-        <v>1813</v>
-      </c>
+      <c r="A1814" s="5"/>
     </row>
     <row r="1815" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1815" s="5">
-        <v>1814</v>
-      </c>
+      <c r="A1815" s="5"/>
     </row>
     <row r="1816" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1816" s="5">
-        <v>1815</v>
-      </c>
+      <c r="A1816" s="5"/>
     </row>
     <row r="1817" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1817" s="5">
-        <v>1816</v>
-      </c>
+      <c r="A1817" s="5"/>
     </row>
     <row r="1818" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1818" s="5">
-        <v>1817</v>
-      </c>
+      <c r="A1818" s="5"/>
     </row>
     <row r="1819" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1819" s="5">
-        <v>1818</v>
-      </c>
+      <c r="A1819" s="5"/>
     </row>
     <row r="1820" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1820" s="5">
-        <v>1819</v>
-      </c>
+      <c r="A1820" s="5"/>
     </row>
     <row r="1821" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1821" s="5">
-        <v>1820</v>
-      </c>
+      <c r="A1821" s="5"/>
     </row>
     <row r="1822" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1822" s="5">
-        <v>1821</v>
-      </c>
+      <c r="A1822" s="5"/>
     </row>
     <row r="1823" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1823" s="5">
-        <v>1822</v>
-      </c>
+      <c r="A1823" s="5"/>
     </row>
     <row r="1824" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1824" s="5">
-        <v>1823</v>
-      </c>
+      <c r="A1824" s="5"/>
     </row>
     <row r="1825" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1825" s="5">
-        <v>1824</v>
-      </c>
+      <c r="A1825" s="5"/>
     </row>
     <row r="1826" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1826" s="5">
-        <v>1825</v>
-      </c>
+      <c r="A1826" s="5"/>
     </row>
     <row r="1827" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1827" s="5">
-        <v>1826</v>
-      </c>
+      <c r="A1827" s="5"/>
     </row>
     <row r="1828" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1828" s="5">
-        <v>1827</v>
-      </c>
+      <c r="A1828" s="5"/>
     </row>
     <row r="1829" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1829" s="5">
-        <v>1828</v>
-      </c>
+      <c r="A1829" s="5"/>
     </row>
     <row r="1830" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1830" s="5">
-        <v>1829</v>
-      </c>
+      <c r="A1830" s="5"/>
     </row>
     <row r="1831" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1831" s="5">
-        <v>1830</v>
-      </c>
+      <c r="A1831" s="5"/>
     </row>
     <row r="1832" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1832" s="5">
-        <v>1831</v>
-      </c>
+      <c r="A1832" s="5"/>
     </row>
     <row r="1833" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1833" s="5">
-        <v>1832</v>
-      </c>
+      <c r="A1833" s="5"/>
     </row>
     <row r="1834" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1834" s="5">
-        <v>1833</v>
-      </c>
+      <c r="A1834" s="5"/>
     </row>
     <row r="1835" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1835" s="5">
-        <v>1834</v>
-      </c>
+      <c r="A1835" s="5"/>
     </row>
     <row r="1836" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1836" s="5">
-        <v>1835</v>
-      </c>
+      <c r="A1836" s="5"/>
     </row>
     <row r="1837" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1837" s="5">
-        <v>1836</v>
-      </c>
+      <c r="A1837" s="5"/>
     </row>
     <row r="1838" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1838" s="5">
-        <v>1837</v>
-      </c>
+      <c r="A1838" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>